<commit_message>
fix: Criando tela de login
</commit_message>
<xml_diff>
--- a/Doc.xlsx
+++ b/Doc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projetos\ecommerce\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B613906-0DF1-4F14-8D95-F171A9BF64E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D1891E0-C596-4BAD-8532-C2E4127ABBB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{F1093086-6291-4AA2-83BA-654D80282985}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
   <si>
     <t>API</t>
   </si>
@@ -38,9 +38,6 @@
   </si>
   <si>
     <t>Na listagem dos usuário, trazer apenas as informações necessárias para realizar a listagem dos itens</t>
-  </si>
-  <si>
-    <t>O Sistema deve identificar quantas vezes o usuário errou a senha e bloquear caso o mesmo tenha tentado uma quantidade de vezes (5 vezes)</t>
   </si>
   <si>
     <t>Criar Endpoint para recuperar a senha</t>
@@ -93,16 +90,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -132,8 +126,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{70F493FA-100E-40B9-ACDD-D7DD134FB4BA}" name="Tabela1" displayName="Tabela1" ref="B2:C7" totalsRowShown="0">
-  <autoFilter ref="B2:C7" xr:uid="{70F493FA-100E-40B9-ACDD-D7DD134FB4BA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{70F493FA-100E-40B9-ACDD-D7DD134FB4BA}" name="Tabela1" displayName="Tabela1" ref="B2:C6" totalsRowShown="0">
+  <autoFilter ref="B2:C6" xr:uid="{70F493FA-100E-40B9-ACDD-D7DD134FB4BA}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{766FB8B5-41C3-4A32-BCE4-413EC2AE7C0B}" name="API" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{B360D7E1-DD1C-4D55-9BD8-583C257876B7}" name="Demanda" dataDxfId="0"/>
@@ -451,10 +445,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63BC806B-5EAF-45F6-8A2B-13B2FB034C47}">
-  <dimension ref="B2:C7"/>
+  <dimension ref="B2:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -484,7 +478,7 @@
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -502,14 +496,6 @@
       </c>
       <c r="C6" s="1" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>